<commit_message>
updated - bug fixes in contract
</commit_message>
<xml_diff>
--- a/buildings.xlsx
+++ b/buildings.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19310"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maristuser\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kulvinder\OneDrive\Documents\Computer Science\Honors Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_EEC7ED7736E12609B980D8720D5E66B37B538D4F" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{2C9A2D0B-0175-4BD3-BA35-7D692E476023}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{AB450CE8-6F6E-486F-9E54-D8204605DDC8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Building Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Assigned</t>
   </si>
   <si>
-    <t>Threshold</t>
-  </si>
-  <si>
     <t>Gartland 1</t>
   </si>
   <si>
@@ -79,13 +76,25 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>Threshold (Winter)</t>
+  </si>
+  <si>
+    <t>Threshold (Summer)</t>
+  </si>
+  <si>
+    <t>Threshold (Spring)</t>
+  </si>
+  <si>
+    <t>Battery Capacity (Spring &amp; Spoof)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,21 +416,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,12 +451,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>22500</v>
@@ -467,10 +486,22 @@
         <f>E2</f>
         <v>425249.99999999994</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2">
+        <v>60059</v>
+      </c>
+      <c r="H2">
+        <v>60208</v>
+      </c>
+      <c r="I2">
+        <v>55208</v>
+      </c>
+      <c r="J2">
+        <v>403393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>22500</v>
@@ -491,10 +522,22 @@
         <f t="shared" ref="F3:F11" si="3">E3</f>
         <v>425249.99999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3">
+        <v>60059</v>
+      </c>
+      <c r="H3">
+        <v>60208</v>
+      </c>
+      <c r="I3">
+        <v>55208</v>
+      </c>
+      <c r="J3">
+        <v>403393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>22500</v>
@@ -515,10 +558,22 @@
         <f t="shared" si="3"/>
         <v>425249.99999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4">
+        <v>60059</v>
+      </c>
+      <c r="H4">
+        <v>60208</v>
+      </c>
+      <c r="I4">
+        <v>55208</v>
+      </c>
+      <c r="J4">
+        <v>403393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>13500</v>
@@ -539,10 +594,22 @@
         <f t="shared" si="3"/>
         <v>255149.99999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5">
+        <v>36035</v>
+      </c>
+      <c r="H5">
+        <v>36124</v>
+      </c>
+      <c r="I5">
+        <v>33365</v>
+      </c>
+      <c r="J5">
+        <v>242036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>13500</v>
@@ -563,10 +630,22 @@
         <f t="shared" si="3"/>
         <v>255149.99999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6">
+        <v>36035</v>
+      </c>
+      <c r="H6">
+        <v>36124</v>
+      </c>
+      <c r="I6">
+        <v>33365</v>
+      </c>
+      <c r="J6">
+        <v>242036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>13500</v>
@@ -587,10 +666,22 @@
         <f t="shared" si="3"/>
         <v>255149.99999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7">
+        <v>36035</v>
+      </c>
+      <c r="H7">
+        <v>36124</v>
+      </c>
+      <c r="I7">
+        <v>33365</v>
+      </c>
+      <c r="J7">
+        <v>242036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>31500</v>
@@ -611,10 +702,22 @@
         <f t="shared" si="3"/>
         <v>595350</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8">
+        <v>84083</v>
+      </c>
+      <c r="H8">
+        <v>84291</v>
+      </c>
+      <c r="I8">
+        <v>77852</v>
+      </c>
+      <c r="J8">
+        <v>564741</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>33000</v>
@@ -635,10 +738,22 @@
         <f t="shared" si="3"/>
         <v>623700</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9">
+        <v>88087</v>
+      </c>
+      <c r="H9">
+        <v>88305</v>
+      </c>
+      <c r="I9">
+        <v>81559</v>
+      </c>
+      <c r="J9">
+        <v>591643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>28000</v>
@@ -659,10 +774,22 @@
         <f t="shared" si="3"/>
         <v>529200</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10">
+        <v>74740</v>
+      </c>
+      <c r="H10">
+        <v>74925</v>
+      </c>
+      <c r="I10">
+        <v>69201</v>
+      </c>
+      <c r="J10">
+        <v>502000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>38000</v>
@@ -683,10 +810,22 @@
         <f t="shared" si="3"/>
         <v>718200</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11">
+        <v>101433</v>
+      </c>
+      <c r="H11">
+        <v>101685</v>
+      </c>
+      <c r="I11">
+        <v>93916</v>
+      </c>
+      <c r="J11">
+        <v>681286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
         <f>SUM(B2:B11)</f>
@@ -707,6 +846,22 @@
       <c r="F12" s="3">
         <f>SUM(F2:F11)</f>
         <v>4507650</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" ref="G12:J12" si="4">SUM(G2:G11)</f>
+        <v>636625</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="4"/>
+        <v>638202</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="4"/>
+        <v>588247</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="4"/>
+        <v>4275957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>